<commit_message>
subo archivos xlsx actualizados
</commit_message>
<xml_diff>
--- a/libmasys/excel/Amor.xlsx
+++ b/libmasys/excel/Amor.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="406">
   <si>
     <t>Titulo</t>
   </si>
@@ -584,13 +584,658 @@
   </si>
   <si>
     <t>AM E 51</t>
+  </si>
+  <si>
+    <t>Cine azul</t>
+  </si>
+  <si>
+    <t>Terry Sothern</t>
+  </si>
+  <si>
+    <t>Edasa</t>
+  </si>
+  <si>
+    <t>AM E 52</t>
+  </si>
+  <si>
+    <t>Epílogo a las Mil y una noches</t>
+  </si>
+  <si>
+    <t>Sir Richard F. Burton</t>
+  </si>
+  <si>
+    <t>Laertes</t>
+  </si>
+  <si>
+    <t>AM E 53</t>
+  </si>
+  <si>
+    <t>Esclava del deseo</t>
+  </si>
+  <si>
+    <t>Johanna Lindsey</t>
+  </si>
+  <si>
+    <t>RBA</t>
+  </si>
+  <si>
+    <t>AM E 54</t>
+  </si>
+  <si>
+    <t>Las amistades peligrosas</t>
+  </si>
+  <si>
+    <t>Choderlos de Laclos</t>
+  </si>
+  <si>
+    <t>AM E 55</t>
+  </si>
+  <si>
+    <t>Las musarañas</t>
+  </si>
+  <si>
+    <t>Eduardo Blanco-Amor</t>
+  </si>
+  <si>
+    <t>Euros</t>
+  </si>
+  <si>
+    <t>AM E 56</t>
+  </si>
+  <si>
+    <t>Madame Bovary</t>
+  </si>
+  <si>
+    <t>Gustave Flaubert</t>
+  </si>
+  <si>
+    <t>Cátedra</t>
+  </si>
+  <si>
+    <t>AM E 57</t>
+  </si>
+  <si>
+    <t>Comer,rezar,amar</t>
+  </si>
+  <si>
+    <t>Elizabeth Gilbert</t>
+  </si>
+  <si>
+    <t>Santillana</t>
+  </si>
+  <si>
+    <t>AM E 58</t>
+  </si>
+  <si>
+    <t>Las naranjas sangrientas</t>
+  </si>
+  <si>
+    <t>John Hawkes</t>
+  </si>
+  <si>
+    <t>Ediciones del Sol</t>
+  </si>
+  <si>
+    <t>AM E 59</t>
+  </si>
+  <si>
+    <t>La doncella</t>
+  </si>
+  <si>
+    <t>Voltaire</t>
+  </si>
+  <si>
+    <t>F. Sempere y Comp.</t>
+  </si>
+  <si>
+    <t>AM E 60</t>
+  </si>
+  <si>
+    <t>Los lenguajes del deseo</t>
+  </si>
+  <si>
+    <t>Enrique Rojas</t>
+  </si>
+  <si>
+    <t>AM E 61</t>
+  </si>
+  <si>
+    <t>Ve a la alcoba a ver si estoy</t>
+  </si>
+  <si>
+    <t>Ángeles López</t>
+  </si>
+  <si>
+    <t>Roger</t>
+  </si>
+  <si>
+    <t>AM E 62</t>
+  </si>
+  <si>
+    <t>La historia de Venus y Tannhäuser</t>
+  </si>
+  <si>
+    <t>Aubrey Beardsley</t>
+  </si>
+  <si>
+    <t>AM E 63</t>
+  </si>
+  <si>
+    <t>Verte desnudo</t>
+  </si>
+  <si>
+    <t>Lourdes Ortiz</t>
+  </si>
+  <si>
+    <t>AM E 64</t>
+  </si>
+  <si>
+    <t>Verte desnuda</t>
+  </si>
+  <si>
+    <t>Antonio Gómez Rufo</t>
+  </si>
+  <si>
+    <t>AM E 65</t>
+  </si>
+  <si>
+    <t>Autodefensa</t>
+  </si>
+  <si>
+    <t>August Strindberg</t>
+  </si>
+  <si>
+    <t>AM E 66</t>
+  </si>
+  <si>
+    <t>La revolución sexual</t>
+  </si>
+  <si>
+    <t>Wilhelm Reich</t>
+  </si>
+  <si>
+    <t>Ruedo Ibérico</t>
+  </si>
+  <si>
+    <t>AM E 67</t>
+  </si>
+  <si>
+    <t>La lucha sexual de los jóvenes</t>
+  </si>
+  <si>
+    <t>Roca</t>
+  </si>
+  <si>
+    <t>AM E 68</t>
+  </si>
+  <si>
+    <t>La prodigiosa isla de las damas</t>
+  </si>
+  <si>
+    <t>Gerhart Hauptmann</t>
+  </si>
+  <si>
+    <t>Rueda</t>
+  </si>
+  <si>
+    <t>AM E 69</t>
+  </si>
+  <si>
+    <t>Grushenka. Tres veces mujer</t>
+  </si>
+  <si>
+    <t>Paul J. Gillette</t>
+  </si>
+  <si>
+    <t>AM E 70</t>
+  </si>
+  <si>
+    <t>El fin del sexo</t>
+  </si>
+  <si>
+    <t>George Leonard</t>
+  </si>
+  <si>
+    <t>Integral</t>
+  </si>
+  <si>
+    <t>AM E 71</t>
+  </si>
+  <si>
+    <t>Delta de Venus</t>
+  </si>
+  <si>
+    <t>Anaïs Nin</t>
+  </si>
+  <si>
+    <t>AM E 72</t>
+  </si>
+  <si>
+    <t>La Antijustina</t>
+  </si>
+  <si>
+    <t>Restif de la Bretonne</t>
+  </si>
+  <si>
+    <t>AM E 73</t>
+  </si>
+  <si>
+    <t>La Gala</t>
+  </si>
+  <si>
+    <t>Marian Izaguirre</t>
+  </si>
+  <si>
+    <t>Torremozas</t>
+  </si>
+  <si>
+    <t>AM E 74</t>
+  </si>
+  <si>
+    <t>Han cortado los laureles</t>
+  </si>
+  <si>
+    <t>Edouard Dujardin</t>
+  </si>
+  <si>
+    <t>Alianza</t>
+  </si>
+  <si>
+    <t>AM E 75</t>
+  </si>
+  <si>
+    <t>El cartero de Neruda</t>
+  </si>
+  <si>
+    <t>Antonio Skarmeta</t>
+  </si>
+  <si>
+    <t>AM E 76</t>
+  </si>
+  <si>
+    <t>El último tango en París</t>
+  </si>
+  <si>
+    <t>Robert Alley</t>
+  </si>
+  <si>
+    <t>AM E 77</t>
+  </si>
+  <si>
+    <t>La vida sexual de Robinson Crusoe</t>
+  </si>
+  <si>
+    <t>Michel Gall</t>
+  </si>
+  <si>
+    <t>AM E 78</t>
+  </si>
+  <si>
+    <t>El Abad C</t>
+  </si>
+  <si>
+    <t>George Bataille</t>
+  </si>
+  <si>
+    <t>Premiá Editora</t>
+  </si>
+  <si>
+    <t>AM E 79</t>
+  </si>
+  <si>
+    <t>Dos noches de placer</t>
+  </si>
+  <si>
+    <t>A. De Musset</t>
+  </si>
+  <si>
+    <t>Editorial Seleción</t>
+  </si>
+  <si>
+    <t>AM E 80</t>
+  </si>
+  <si>
+    <t>Nuevas cartas portuguesas</t>
+  </si>
+  <si>
+    <t>Mariana de Alcoforado</t>
+  </si>
+  <si>
+    <t>AM E 81</t>
+  </si>
+  <si>
+    <t>La vida después</t>
+  </si>
+  <si>
+    <t>Marta Rivera de la Cruz</t>
+  </si>
+  <si>
+    <t>AM E 82</t>
+  </si>
+  <si>
+    <t>La inglesa romántica</t>
+  </si>
+  <si>
+    <t>Thomas Wiseman</t>
+  </si>
+  <si>
+    <t>Sudamericana</t>
+  </si>
+  <si>
+    <t>AM E 83</t>
+  </si>
+  <si>
+    <t>Primer amor</t>
+  </si>
+  <si>
+    <t>Samuel Beckett</t>
+  </si>
+  <si>
+    <t>AM E 84</t>
+  </si>
+  <si>
+    <t>La fuente enterrada</t>
+  </si>
+  <si>
+    <t>Carmen de Içaza</t>
+  </si>
+  <si>
+    <t>AM E 85</t>
+  </si>
+  <si>
+    <t>Las consecuencias del amor</t>
+  </si>
+  <si>
+    <t>Sulaiman Addonia</t>
+  </si>
+  <si>
+    <t>AM E 86</t>
+  </si>
+  <si>
+    <t>Estado de excitación</t>
+  </si>
+  <si>
+    <t>Ethan Hawke</t>
+  </si>
+  <si>
+    <t>AM E 87</t>
+  </si>
+  <si>
+    <t>La transformación de la intimidad</t>
+  </si>
+  <si>
+    <t>Anthony Giddens</t>
+  </si>
+  <si>
+    <t>AM E 88</t>
+  </si>
+  <si>
+    <t>Brújula para navegantes emocionales</t>
+  </si>
+  <si>
+    <t>Elsa Punset</t>
+  </si>
+  <si>
+    <t>AM E 89</t>
+  </si>
+  <si>
+    <t>Espirita</t>
+  </si>
+  <si>
+    <t>Téophile Gautier</t>
+  </si>
+  <si>
+    <t>Edhasa</t>
+  </si>
+  <si>
+    <t>AM E 90</t>
+  </si>
+  <si>
+    <t>La pasión turca</t>
+  </si>
+  <si>
+    <t>Antonio Gala</t>
+  </si>
+  <si>
+    <t>AM E 91</t>
+  </si>
+  <si>
+    <t>Hermana de fuego</t>
+  </si>
+  <si>
+    <t>Jude Deveraux</t>
+  </si>
+  <si>
+    <t>AM E 92</t>
+  </si>
+  <si>
+    <t>Sed de amor</t>
+  </si>
+  <si>
+    <t>Kresley Cole</t>
+  </si>
+  <si>
+    <t>AM E 93</t>
+  </si>
+  <si>
+    <t>Placeres</t>
+  </si>
+  <si>
+    <t>Lonnie Barbach</t>
+  </si>
+  <si>
+    <t>AM E 94</t>
+  </si>
+  <si>
+    <t>Espera, ponte así</t>
+  </si>
+  <si>
+    <t>Andreu Martín</t>
+  </si>
+  <si>
+    <t>AM E 95</t>
+  </si>
+  <si>
+    <t>Bestiario de amor</t>
+  </si>
+  <si>
+    <t>Richard de Fournival</t>
+  </si>
+  <si>
+    <t>Miraguano Ediciones</t>
+  </si>
+  <si>
+    <t>AM E 96</t>
+  </si>
+  <si>
+    <t>El hombre de cincuenta años</t>
+  </si>
+  <si>
+    <t>Goethe y otros</t>
+  </si>
+  <si>
+    <t>Alba</t>
+  </si>
+  <si>
+    <t>AM E 97</t>
+  </si>
+  <si>
+    <t>Breve historia del sexo</t>
+  </si>
+  <si>
+    <t>Béatrice Bantman</t>
+  </si>
+  <si>
+    <t>Paidós</t>
+  </si>
+  <si>
+    <t>AM E 98</t>
+  </si>
+  <si>
+    <t>El hombre negro</t>
+  </si>
+  <si>
+    <t>Carmen de Burgos</t>
+  </si>
+  <si>
+    <t>Emiliano Escolar Editor</t>
+  </si>
+  <si>
+    <t>AM E 99</t>
+  </si>
+  <si>
+    <t>Afrodita</t>
+  </si>
+  <si>
+    <t>Isabel Allende</t>
+  </si>
+  <si>
+    <t>AM E 100</t>
+  </si>
+  <si>
+    <t>Diario de un seductor</t>
+  </si>
+  <si>
+    <t>Sören Kierkegaard</t>
+  </si>
+  <si>
+    <t>AM E 101</t>
+  </si>
+  <si>
+    <t>Memorias de una pulga</t>
+  </si>
+  <si>
+    <t>Ramón Ricardo</t>
+  </si>
+  <si>
+    <t>AM E 102</t>
+  </si>
+  <si>
+    <t>Tiempo de morir</t>
+  </si>
+  <si>
+    <t>Louis Aragon</t>
+  </si>
+  <si>
+    <t>AM E 103</t>
+  </si>
+  <si>
+    <t>Teleny</t>
+  </si>
+  <si>
+    <t>Oscar Wilde</t>
+  </si>
+  <si>
+    <t>AM E 104</t>
+  </si>
+  <si>
+    <t>La silla vacía</t>
+  </si>
+  <si>
+    <t>Nachman de Breslau</t>
+  </si>
+  <si>
+    <t>Olañeta</t>
+  </si>
+  <si>
+    <t>AM E 105</t>
+  </si>
+  <si>
+    <t>El fondo del vaso</t>
+  </si>
+  <si>
+    <t>Francisco Ayala</t>
+  </si>
+  <si>
+    <t>AM E 106</t>
+  </si>
+  <si>
+    <t>El portero de noche</t>
+  </si>
+  <si>
+    <t>Liliana Cavani</t>
+  </si>
+  <si>
+    <t>Icaria</t>
+  </si>
+  <si>
+    <t>AM E 107</t>
+  </si>
+  <si>
+    <t>Sexualidad en el hombre y en la mujer</t>
+  </si>
+  <si>
+    <t>Theodore Reik</t>
+  </si>
+  <si>
+    <t>Diana</t>
+  </si>
+  <si>
+    <t>AM E 108</t>
+  </si>
+  <si>
+    <t>La necesidad de ser amado</t>
+  </si>
+  <si>
+    <t>AM E 109</t>
+  </si>
+  <si>
+    <t>Psicología de las relaciones sexuales</t>
+  </si>
+  <si>
+    <t>Nova</t>
+  </si>
+  <si>
+    <t>AM E 110</t>
+  </si>
+  <si>
+    <t>Bodas de plata</t>
+  </si>
+  <si>
+    <t>Begoña garcía Diego</t>
+  </si>
+  <si>
+    <t>Madrid</t>
+  </si>
+  <si>
+    <t>AM E 111</t>
+  </si>
+  <si>
+    <t>Las bostonianas</t>
+  </si>
+  <si>
+    <t>Henry James</t>
+  </si>
+  <si>
+    <t>Seix Barral</t>
+  </si>
+  <si>
+    <t>AM E 112</t>
+  </si>
+  <si>
+    <t>Mía para siempre</t>
+  </si>
+  <si>
+    <t>Kathryn Smith</t>
+  </si>
+  <si>
+    <t>AM E 113</t>
+  </si>
+  <si>
+    <t>Dos damas muy serias</t>
+  </si>
+  <si>
+    <t>Jane Bowles</t>
+  </si>
+  <si>
+    <t>AM E 114</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -601,6 +1246,9 @@
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -621,7 +1269,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -630,6 +1278,12 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1701,6 +2355,1267 @@
         <v>190</v>
       </c>
     </row>
+    <row r="53">
+      <c r="A53" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D53" s="2">
+        <v>1971.0</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D54" s="2">
+        <v>1989.0</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D55" s="2">
+        <v>2010.0</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D56" s="2">
+        <v>2002.0</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D57" s="2">
+        <v>1975.0</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D58" s="2">
+        <v>1999.0</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D59" s="2">
+        <v>2009.0</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="D60" s="2">
+        <v>1975.0</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D61" s="2">
+        <v>1933.0</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D62" s="2">
+        <v>2004.0</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D63" s="2">
+        <v>1998.0</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D64" s="2">
+        <v>1998.0</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D65" s="2">
+        <v>1992.0</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D66" s="2">
+        <v>1992.0</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="D67" s="2">
+        <v>1967.0</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D68" s="2">
+        <v>1970.0</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D69" s="2">
+        <v>1974.0</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D70" s="2">
+        <v>1966.0</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="D71" s="2">
+        <v>1968.0</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D72" s="2">
+        <v>1983.0</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="D73" s="2">
+        <v>1978.0</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="D74" s="2">
+        <v>1992.0</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="D75" s="2">
+        <v>1990.0</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D76" s="2">
+        <v>1973.0</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="D77" s="2">
+        <v>2008.0</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="D78" s="2">
+        <v>1973.0</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D79" s="2">
+        <v>1988.0</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="D80" s="2">
+        <v>1977.0</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D81" s="2">
+        <v>1954.0</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D82" s="2">
+        <v>1976.0</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D83" s="2">
+        <v>2001.0</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H83" s="2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="D84" s="2">
+        <v>1975.0</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D85" s="2">
+        <v>1972.0</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H85" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="D86" s="2">
+        <v>2009.0</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="D87" s="2">
+        <v>2009.0</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="D88" s="2">
+        <v>2001.0</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="D89" s="2">
+        <v>1995.0</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="D90" s="2">
+        <v>2009.0</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H90" s="2" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="D91" s="2">
+        <v>1971.0</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H91" s="2" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="D92" s="2">
+        <v>1995.0</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H92" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="D93" s="2">
+        <v>2005.0</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H93" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="D94" s="2">
+        <v>2009.0</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H94" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="D95" s="2">
+        <v>1989.0</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H95" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="D96" s="2">
+        <v>2001.0</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H96" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="D97" s="2">
+        <v>1980.0</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H97" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="D98" s="2">
+        <v>2002.0</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H98" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="D99" s="2">
+        <v>1998.0</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H99" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="D100" s="2">
+        <v>1980.0</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H100" s="2" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="D101" s="2">
+        <v>2003.0</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H101" s="2" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="D102" s="2">
+        <v>1951.0</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H102" s="2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="D103" s="2">
+        <v>1969.0</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H103" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="D104" s="2">
+        <v>1969.0</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H104" s="2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="D105" s="2">
+        <v>1980.0</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H105" s="2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="D106" s="2">
+        <v>1997.0</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H106" s="2" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="D107" s="2">
+        <v>1970.0</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H107" s="2" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="D108" s="2">
+        <v>1976.0</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H108" s="2" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="D109" s="2">
+        <v>1965.0</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H109" s="2" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="D110" s="2">
+        <v>1965.0</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H110" s="2" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="D111" s="2">
+        <v>1955.0</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H111" s="2" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D112" s="2">
+        <v>1958.0</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H112" s="2" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="D113" s="2">
+        <v>1986.0</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H113" s="2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="C114" s="3"/>
+      <c r="D114" s="4">
+        <v>2008.0</v>
+      </c>
+      <c r="E114" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H114" s="2" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="D115" s="2">
+        <v>1989.0</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H115" s="2" t="s">
+        <v>405</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>